<commit_message>
Analysis of Citizens vs. Non-Citizens
</commit_message>
<xml_diff>
--- a/Data/Ukraine Appropriations Breakdown.xlsx
+++ b/Data/Ukraine Appropriations Breakdown.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Owner/Documents/Blog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Owner/Documents/Blog/Ukraine Appropriations Analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB5414F5-DFBD-3B47-99EB-B2F7D271FFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892C74B6-B5A3-3444-BA95-B6F06B491BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="980" windowWidth="27640" windowHeight="15640" xr2:uid="{42D9E657-4673-034D-96AA-B95A893C1F67}"/>
   </bookViews>
@@ -172,9 +172,6 @@
     <t>for the Financial Crimes Enforcement Network (FinCEN) to support development, coordination, implementation, and enforcement of targeted financial measures.</t>
   </si>
   <si>
-    <t>Title VI –</t>
-  </si>
-  <si>
     <t>State, Foreign Operations, and Related Programs</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t>The legislation includes $3 billion in authority to drawdown defense articles and services and increased flexibility to transfer excess defense equipment for Ukraine and other regional allies.</t>
+  </si>
+  <si>
+    <t>Title VI</t>
   </si>
 </sst>
 </file>
@@ -633,7 +633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36214490-E744-1A4E-BA07-02DD9F6A0181}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -869,224 +871,224 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>47</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>48</v>
-      </c>
-      <c r="E14" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
       <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
         <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>51</v>
       </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
       <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
         <v>52</v>
-      </c>
-      <c r="E16" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
       <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
         <v>54</v>
-      </c>
-      <c r="E17" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="C18" t="s">
-        <v>47</v>
-      </c>
       <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
         <v>56</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
         <v>59</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>60</v>
-      </c>
-      <c r="E20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
         <v>62</v>
-      </c>
-      <c r="E21" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
         <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
         <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s">
         <v>67</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>68</v>
-      </c>
-      <c r="E24" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
         <v>70</v>
-      </c>
-      <c r="D25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
         <v>72</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>73</v>
-      </c>
-      <c r="E26" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>